<commit_message>
Intégration des éléments concernant la structure issus du GT Structure (#254)
* Intégration des éléments concernant la structure issus du gt Structure : profiles, extensions, CS, VS, page content, exemples.

* prise en comptes des remarques de la PR

* ajout de la dépendance extensions r5 pour les imports en r4

* changement du template interop-santé

* suppression de l'extension description pour utiliser la propriété description importée de la R5

* changement de la description

* simplification de l'extension

* changement de la contrainte sur le type du profile

* ajout des changements suite à l'intégration des travaux du GT structure

* suppression du CS obsolete

* Update FRCoreOrganizationEtablissementProfile.fsh

* Add organization type and activity sectors to profile

* add slicing

---------

Co-authored-by: Frederic Laurent <laurentfr@chu-rennes.fr>
Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> 01619f71975fedcc96eaf3a22f63a8fbbf7f880b
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-fr-core-cs-location-type.xlsx
+++ b/main/ig/CodeSystem-fr-core-cs-location-type.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -48,7 +48,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-28T09:35:28+00:00</t>
+    <t>2026-01-28T10:29:57+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -144,28 +144,52 @@
     <t>1</t>
   </si>
   <si>
-    <t>PRSN_NGTV</t>
-  </si>
-  <si>
-    <t>Pression négative</t>
-  </si>
-  <si>
-    <t>PRSN_PSTV</t>
-  </si>
-  <si>
-    <t>Pression positive</t>
-  </si>
-  <si>
-    <t>CRCRL</t>
-  </si>
-  <si>
-    <t>Carcéral</t>
-  </si>
-  <si>
-    <t>CPTN</t>
-  </si>
-  <si>
-    <t>Capitonné</t>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>Bâtiment</t>
+  </si>
+  <si>
+    <t>ETAG</t>
+  </si>
+  <si>
+    <t>Étage</t>
+  </si>
+  <si>
+    <t>COUL</t>
+  </si>
+  <si>
+    <t>Couloir</t>
+  </si>
+  <si>
+    <t>AILE</t>
+  </si>
+  <si>
+    <t>Aile</t>
+  </si>
+  <si>
+    <t>BOX</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>CHAMB</t>
+  </si>
+  <si>
+    <t>Chambre</t>
+  </si>
+  <si>
+    <t>LIT</t>
+  </si>
+  <si>
+    <t>lit</t>
+  </si>
+  <si>
+    <t>PL_TECH</t>
+  </si>
+  <si>
+    <t>Plateau technique</t>
   </si>
   <si>
     <t>PNT_CLCT</t>
@@ -180,40 +204,16 @@
     <t>Point de livraison</t>
   </si>
   <si>
-    <t>SL_ATNT</t>
-  </si>
-  <si>
-    <t>Salle d’attente</t>
-  </si>
-  <si>
-    <t>SL_RVL</t>
-  </si>
-  <si>
-    <t>Salle réveil</t>
-  </si>
-  <si>
     <t>SL_EXM</t>
   </si>
   <si>
     <t>Salle examen</t>
   </si>
   <si>
-    <t>SL_RN</t>
-  </si>
-  <si>
-    <t>Salle de réunion</t>
-  </si>
-  <si>
-    <t>SL_TRV</t>
-  </si>
-  <si>
-    <t>Salle de travail</t>
-  </si>
-  <si>
-    <t>ACC</t>
-  </si>
-  <si>
-    <t>Point d'accueil</t>
+    <t>SL_CONS</t>
+  </si>
+  <si>
+    <t>Salle de consultation</t>
   </si>
 </sst>
 </file>
@@ -564,9 +564,7 @@
       <c r="C2" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D2" t="s" s="2">
-        <v>44</v>
-      </c>
+      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
@@ -578,9 +576,7 @@
       <c r="C3" t="s" s="2">
         <v>46</v>
       </c>
-      <c r="D3" t="s" s="2">
-        <v>46</v>
-      </c>
+      <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
@@ -592,9 +588,7 @@
       <c r="C4" t="s" s="2">
         <v>48</v>
       </c>
-      <c r="D4" t="s" s="2">
-        <v>48</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
@@ -606,9 +600,7 @@
       <c r="C5" t="s" s="2">
         <v>50</v>
       </c>
-      <c r="D5" t="s" s="2">
-        <v>50</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
@@ -620,9 +612,7 @@
       <c r="C6" t="s" s="2">
         <v>52</v>
       </c>
-      <c r="D6" t="s" s="2">
-        <v>52</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
@@ -634,9 +624,7 @@
       <c r="C7" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="D7" t="s" s="2">
-        <v>54</v>
-      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
@@ -648,9 +636,7 @@
       <c r="C8" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="D8" t="s" s="2">
-        <v>56</v>
-      </c>
+      <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
@@ -662,9 +648,7 @@
       <c r="C9" t="s" s="2">
         <v>58</v>
       </c>
-      <c r="D9" t="s" s="2">
-        <v>58</v>
-      </c>
+      <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
@@ -676,9 +660,7 @@
       <c r="C10" t="s" s="2">
         <v>60</v>
       </c>
-      <c r="D10" t="s" s="2">
-        <v>60</v>
-      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
@@ -690,9 +672,7 @@
       <c r="C11" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="D11" t="s" s="2">
-        <v>62</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
@@ -704,9 +684,7 @@
       <c r="C12" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="D12" t="s" s="2">
-        <v>64</v>
-      </c>
+      <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
@@ -718,9 +696,7 @@
       <c r="C13" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="D13" t="s" s="2">
-        <v>66</v>
-      </c>
+      <c r="D13" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>